<commit_message>
adding classes in UML class diagram
</commit_message>
<xml_diff>
--- a/template_pegase_v1/chromatography.xlsx
+++ b/template_pegase_v1/chromatography.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -38,12 +38,6 @@
     <t>SampleID</t>
   </si>
   <si>
-    <t>ExtractionType</t>
-  </si>
-  <si>
-    <t>SamplePortion</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -53,9 +47,6 @@
     <t>#string</t>
   </si>
   <si>
-    <t>#float,  unit:µlormg</t>
-  </si>
-  <si>
     <t>#Date format jj/mm/aaa</t>
   </si>
   <si>
@@ -78,12 +69,6 @@
   </si>
   <si>
     <t>#Identifiant de l'echantillon</t>
-  </si>
-  <si>
-    <t>#TypeExtraction</t>
-  </si>
-  <si>
-    <t>#PriseEssai</t>
   </si>
   <si>
     <t>#Commentaire</t>
@@ -131,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -165,81 +150,63 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>